<commit_message>
Daily attendance update - 2025-08-13
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC9964B-13A0-46B5-863A-F2BD61060F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE269317-49F3-4951-B377-E9A63CF62A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Feb" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -5658,8 +5658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F16C68-A443-46CF-B7FA-2968469C0FB5}">
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5924,8 +5924,12 @@
       <c r="P3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+      <c r="Q3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="S3" s="2"/>
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
@@ -6059,8 +6063,12 @@
       <c r="P5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
+      <c r="Q5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="S5" s="2"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
@@ -6209,8 +6217,12 @@
       <c r="P7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
+      <c r="Q7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="S7" s="2"/>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
@@ -6285,7 +6297,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AJ3,"WFO")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AJ3,"WFH")</f>
@@ -6311,11 +6323,11 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -6337,7 +6349,7 @@
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Daily attendance update - 2025-08-14
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA2202E-7C1C-4166-B8F8-265EB8F73E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC3B7B5-FAF0-4E45-B0C1-2F22182C1B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -848,30 +848,30 @@
       <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -972,7 +972,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1063,7 +1063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1542,28 +1542,28 @@
       <selection pane="topRight" activeCell="AC6" sqref="AC6:AG6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>45747</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1773,7 +1773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="AI4" s="2"/>
       <c r="AJ4" s="13"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="AI5" s="2"/>
       <c r="AJ5" s="13"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2127,7 +2127,7 @@
       <c r="AI6" s="2"/>
       <c r="AJ6" s="13"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2215,7 +2215,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="13"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2253,7 +2253,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="14"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -2360,29 +2360,29 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2586,7 +2586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3078,7 +3078,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -3185,29 +3185,29 @@
       <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>45808</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3417,7 +3417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -3601,7 +3601,7 @@
       </c>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3877,7 +3877,7 @@
       </c>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3914,7 +3914,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -4025,15 +4025,15 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4237,7 +4237,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -4719,7 +4719,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -4827,17 +4827,17 @@
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>45869</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5047,7 +5047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -5554,7 +5554,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -5659,20 +5659,21 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3:T7"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -5783,7 +5784,7 @@
       </c>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5883,7 +5884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5930,7 +5931,9 @@
       <c r="R3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="2"/>
+      <c r="S3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="T3" s="6" t="s">
         <v>25</v>
       </c>
@@ -5950,7 +5953,7 @@
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -6026,7 +6029,7 @@
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -6073,7 +6076,9 @@
       <c r="R5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="2"/>
+      <c r="S5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="T5" s="6" t="s">
         <v>25</v>
       </c>
@@ -6094,7 +6099,7 @@
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -6184,7 +6189,7 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -6231,7 +6236,9 @@
       <c r="R7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S7" s="2"/>
+      <c r="S7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="T7" s="6" t="s">
         <v>25</v>
       </c>
@@ -6252,7 +6259,7 @@
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6290,7 +6297,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -6301,7 +6308,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -6311,10 +6318,10 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AJ3,"WFH")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -6327,7 +6334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -6337,10 +6344,10 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -6353,7 +6360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -6363,7 +6370,7 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-08-21
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC3B7B5-FAF0-4E45-B0C1-2F22182C1B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E37C5A-BE00-4704-97EF-ADDFCCA5E7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Feb" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -848,30 +848,30 @@
       <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -972,7 +972,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1063,7 +1063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1542,28 +1542,28 @@
       <selection pane="topRight" activeCell="AC6" sqref="AC6:AG6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>45747</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1773,7 +1773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="AI4" s="2"/>
       <c r="AJ4" s="13"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="AI5" s="2"/>
       <c r="AJ5" s="13"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2127,7 +2127,7 @@
       <c r="AI6" s="2"/>
       <c r="AJ6" s="13"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2215,7 +2215,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="13"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2253,7 +2253,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="14"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -2360,29 +2360,29 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2586,7 +2586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3078,7 +3078,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -3185,29 +3185,29 @@
       <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>45808</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3417,7 +3417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -3601,7 +3601,7 @@
       </c>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3877,7 +3877,7 @@
       </c>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3914,7 +3914,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -4025,15 +4025,15 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4237,7 +4237,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -4719,7 +4719,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -4827,17 +4827,17 @@
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>45869</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5047,7 +5047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -5554,7 +5554,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -5659,21 +5659,21 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -5784,7 +5784,7 @@
       </c>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5884,7 +5884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5939,10 +5939,21 @@
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
+      <c r="W3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AB3" s="7"/>
       <c r="AC3" s="7"/>
       <c r="AD3" s="2"/>
@@ -5953,7 +5964,7 @@
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -6017,7 +6028,9 @@
       <c r="Y4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Z4" s="2"/>
+      <c r="Z4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
@@ -6029,7 +6042,7 @@
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -6084,10 +6097,18 @@
       </c>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
+      <c r="W5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AA5" s="2"/>
       <c r="AB5" s="7"/>
       <c r="AC5" s="7"/>
@@ -6099,7 +6120,7 @@
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -6189,7 +6210,7 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -6244,10 +6265,18 @@
       </c>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
+      <c r="W7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
@@ -6259,7 +6288,7 @@
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6297,7 +6326,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -6308,46 +6337,46 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AJ3,"WFO")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AJ3,"WFH")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14:B17" si="0">COUNTIF(F4:AJ4,"WFO")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" ref="C14:C17" si="1">COUNTIF(F4:AJ4,"WFH")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -6360,17 +6389,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-08-22
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C7B215-E652-42F2-BE7D-BECFBB55662F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46A941C-2E60-4A4C-A6B5-071231319C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Feb" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -5659,7 +5659,7 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6031,7 +6031,9 @@
       <c r="Z4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AA4" s="2"/>
+      <c r="AA4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
       <c r="AD4" s="2"/>
@@ -6109,7 +6111,9 @@
       <c r="Z5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AA5" s="2"/>
+      <c r="AA5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AB5" s="7"/>
       <c r="AC5" s="7"/>
       <c r="AD5" s="2"/>
@@ -6277,7 +6281,9 @@
       <c r="Z7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AA7" s="2"/>
+      <c r="AA7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
       <c r="AD7" s="2"/>
@@ -6356,7 +6362,7 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14:B17" si="0">COUNTIF(F4:AJ4,"WFO")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" ref="C14:C17" si="1">COUNTIF(F4:AJ4,"WFH")</f>
@@ -6373,7 +6379,7 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
@@ -6399,7 +6405,7 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-08-25
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46A941C-2E60-4A4C-A6B5-071231319C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8106D442-92F7-40BB-A8C7-9060E7181060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Feb" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -848,30 +848,30 @@
       <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -972,7 +972,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1063,7 +1063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1542,28 +1542,28 @@
       <selection pane="topRight" activeCell="AC6" sqref="AC6:AG6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>45747</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1773,7 +1773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="AI4" s="2"/>
       <c r="AJ4" s="13"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="AI5" s="2"/>
       <c r="AJ5" s="13"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2127,7 +2127,7 @@
       <c r="AI6" s="2"/>
       <c r="AJ6" s="13"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2215,7 +2215,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="13"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2253,7 +2253,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="14"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -2360,29 +2360,29 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2586,7 +2586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3078,7 +3078,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -3185,29 +3185,29 @@
       <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>45808</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3417,7 +3417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -3601,7 +3601,7 @@
       </c>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3877,7 +3877,7 @@
       </c>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3914,7 +3914,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -4025,15 +4025,15 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4237,7 +4237,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -4719,7 +4719,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -4827,17 +4827,17 @@
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>45869</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5047,7 +5047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -5554,7 +5554,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -5658,22 +5658,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F16C68-A443-46CF-B7FA-2968469C0FB5}">
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -5784,7 +5784,7 @@
       </c>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5884,7 +5884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5956,7 +5956,9 @@
       </c>
       <c r="AB3" s="7"/>
       <c r="AC3" s="7"/>
-      <c r="AD3" s="2"/>
+      <c r="AD3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
@@ -5964,7 +5966,7 @@
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -6036,7 +6038,9 @@
       </c>
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
-      <c r="AD4" s="2"/>
+      <c r="AD4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
@@ -6044,7 +6048,7 @@
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -6116,7 +6120,9 @@
       </c>
       <c r="AB5" s="7"/>
       <c r="AC5" s="7"/>
-      <c r="AD5" s="2"/>
+      <c r="AD5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
@@ -6124,7 +6130,7 @@
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -6214,7 +6220,7 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -6286,7 +6292,9 @@
       </c>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
-      <c r="AD7" s="2"/>
+      <c r="AD7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
@@ -6294,7 +6302,7 @@
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6332,7 +6340,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -6343,46 +6351,46 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AJ3,"WFO")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AJ3,"WFH")</f>
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14:B17" si="0">COUNTIF(F4:AJ4,"WFO")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" ref="C14:C17" si="1">COUNTIF(F4:AJ4,"WFH")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -6395,13 +6403,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Daily attendance update - 2025-08-26
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8106D442-92F7-40BB-A8C7-9060E7181060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338D7D90-0E44-4780-9644-C8F9DCC48B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Feb" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -848,30 +848,30 @@
       <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -972,7 +972,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1063,7 +1063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1542,28 +1542,28 @@
       <selection pane="topRight" activeCell="AC6" sqref="AC6:AG6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>45747</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1773,7 +1773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1951,7 +1951,7 @@
       <c r="AI4" s="2"/>
       <c r="AJ4" s="13"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="AI5" s="2"/>
       <c r="AJ5" s="13"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2127,7 +2127,7 @@
       <c r="AI6" s="2"/>
       <c r="AJ6" s="13"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2215,7 +2215,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="13"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2253,7 +2253,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="14"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -2360,29 +2360,29 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2586,7 +2586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3078,7 +3078,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -3185,29 +3185,29 @@
       <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>45808</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3417,7 +3417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -3601,7 +3601,7 @@
       </c>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3877,7 +3877,7 @@
       </c>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3914,7 +3914,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -4025,15 +4025,15 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4237,7 +4237,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -4504,7 +4504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -4719,7 +4719,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -4827,17 +4827,17 @@
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>45869</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5047,7 +5047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -5554,7 +5554,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -5604,7 +5604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -5658,22 +5658,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F16C68-A443-46CF-B7FA-2968469C0FB5}">
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3:AF7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -5784,7 +5784,7 @@
       </c>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5884,7 +5884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5959,14 +5959,18 @@
       <c r="AD3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
+      <c r="AE3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -6041,14 +6045,18 @@
       <c r="AD4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
+      <c r="AE4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -6123,14 +6131,18 @@
       <c r="AD5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AE5" s="2"/>
-      <c r="AF5" s="2"/>
+      <c r="AE5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF5" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -6209,7 +6221,7 @@
         <v>24</v>
       </c>
       <c r="AF6" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AG6" s="6" t="s">
         <v>24</v>
@@ -6220,7 +6232,7 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -6295,14 +6307,18 @@
       <c r="AD7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
+      <c r="AE7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF7" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6340,7 +6356,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -6351,33 +6367,33 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AJ3,"WFO")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AJ3,"WFH")</f>
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14:B17" si="0">COUNTIF(F4:AJ4,"WFO")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" ref="C14:C17" si="1">COUNTIF(F4:AJ4,"WFH")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -6387,10 +6403,10 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -6403,13 +6419,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Daily attendance update - 2025-08-28
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338D7D90-0E44-4780-9644-C8F9DCC48B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FD09A9-503C-4268-87B5-C20A183ABEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -5659,7 +5659,7 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3:AF7"/>
+      <selection activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5965,7 +5965,9 @@
       <c r="AF3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AG3" s="2"/>
+      <c r="AG3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AH3" s="2"/>
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
@@ -6051,7 +6053,9 @@
       <c r="AF4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AG4" s="2"/>
+      <c r="AG4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AH4" s="2"/>
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
@@ -6137,7 +6141,9 @@
       <c r="AF5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AG5" s="2"/>
+      <c r="AG5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AH5" s="2"/>
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
@@ -6313,7 +6319,9 @@
       <c r="AF7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AG7" s="2"/>
+      <c r="AG7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AH7" s="2"/>
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
@@ -6377,7 +6385,7 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AJ3,"WFH")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -6386,7 +6394,7 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14:B17" si="0">COUNTIF(F4:AJ4,"WFO")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" ref="C14:C17" si="1">COUNTIF(F4:AJ4,"WFH")</f>
@@ -6399,7 +6407,7 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
@@ -6425,7 +6433,7 @@
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-01
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FD09A9-503C-4268-87B5-C20A183ABEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DC3B20-4339-4224-932C-C1D72B77874D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" firstSheet="5" activeTab="7" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Feb" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="UV-WMS Admin June" sheetId="5" r:id="rId5"/>
     <sheet name="UV-WMS Admin July" sheetId="6" r:id="rId6"/>
     <sheet name="UV-WMS Admin August" sheetId="7" r:id="rId7"/>
+    <sheet name="UV-WMS Admin September" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -350,7 +351,37 @@
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2339,10 +2370,10 @@
     <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:B15">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3164,10 +3195,10 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4000,15 +4031,15 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4805,13 +4836,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5640,13 +5671,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5658,8 +5689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F16C68-A443-46CF-B7FA-2968469C0FB5}">
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AG7" sqref="AG7"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S14" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5968,7 +5999,9 @@
       <c r="AG3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AH3" s="2"/>
+      <c r="AH3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
     </row>
@@ -6056,7 +6089,9 @@
       <c r="AG4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AH4" s="2"/>
+      <c r="AH4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
     </row>
@@ -6144,7 +6179,9 @@
       <c r="AG5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AH5" s="2"/>
+      <c r="AH5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
     </row>
@@ -6322,7 +6359,9 @@
       <c r="AG7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AH7" s="2"/>
+      <c r="AH7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
     </row>
@@ -6385,7 +6424,7 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AJ3,"WFH")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
@@ -6398,7 +6437,7 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ref="C14:C17" si="1">COUNTIF(F4:AJ4,"WFH")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
@@ -6407,7 +6446,7 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="1"/>
@@ -6437,7 +6476,618 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="B13:B17">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7CEAED-F464-426C-A766-484A87191C7F}">
+  <dimension ref="A1:AI17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>45901</v>
+      </c>
+      <c r="G1" s="1">
+        <v>45902</v>
+      </c>
+      <c r="H1" s="1">
+        <v>45903</v>
+      </c>
+      <c r="I1" s="1">
+        <v>45904</v>
+      </c>
+      <c r="J1" s="1">
+        <v>45905</v>
+      </c>
+      <c r="K1" s="1">
+        <v>45906</v>
+      </c>
+      <c r="L1" s="1">
+        <v>45907</v>
+      </c>
+      <c r="M1" s="1">
+        <v>45908</v>
+      </c>
+      <c r="N1" s="1">
+        <v>45909</v>
+      </c>
+      <c r="O1" s="1">
+        <v>45910</v>
+      </c>
+      <c r="P1" s="1">
+        <v>45911</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>45912</v>
+      </c>
+      <c r="R1" s="1">
+        <v>45913</v>
+      </c>
+      <c r="S1" s="1">
+        <v>45914</v>
+      </c>
+      <c r="T1" s="1">
+        <v>45915</v>
+      </c>
+      <c r="U1" s="1">
+        <v>45916</v>
+      </c>
+      <c r="V1" s="1">
+        <v>45917</v>
+      </c>
+      <c r="W1" s="1">
+        <v>45918</v>
+      </c>
+      <c r="X1" s="1">
+        <v>45919</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>45920</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>45921</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>45922</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>45923</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>45924</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>45925</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>45926</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>45927</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>45928</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>45929</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>45930</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>35898</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2">
+        <v>33548</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44429</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
+        <v>36698</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45078</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <f>COUNTIF(F3:AI3,"WFO")</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <f>COUNTIF(F3:AI3,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <f>COUNTIF(F4:AI4,"WFO")</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <f>COUNTIF(F4:AI4,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2">
+        <f>COUNTIF(F5:AI5,"WFO")</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <f>COUNTIF(F5:AI5,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2">
+        <f>COUNTIF(F6:AI6,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <f>COUNTIF(F6:AI6,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2">
+        <f>COUNTIF(F7:AI7,"WFO")</f>
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <f>COUNTIF(F7:AI7,"WFH")</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-04
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DC3B20-4339-4224-932C-C1D72B77874D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACC3C17-E1A9-4B85-9AB5-040D4943C3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" firstSheet="5" activeTab="7" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
-    <sheet name="UV-WMS Admin Feb" sheetId="1" r:id="rId1"/>
-    <sheet name="UV-WMS Admin March" sheetId="2" r:id="rId2"/>
-    <sheet name="UV-WMS Admin April" sheetId="3" r:id="rId3"/>
-    <sheet name="UV-WMS Admin May" sheetId="4" r:id="rId4"/>
-    <sheet name="UV-WMS Admin June" sheetId="5" r:id="rId5"/>
-    <sheet name="UV-WMS Admin July" sheetId="6" r:id="rId6"/>
-    <sheet name="UV-WMS Admin August" sheetId="7" r:id="rId7"/>
-    <sheet name="UV-WMS Admin September" sheetId="8" r:id="rId8"/>
+    <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
+    <sheet name="UV-WMS Admin Feb" sheetId="1" r:id="rId2"/>
+    <sheet name="UV-WMS Admin March" sheetId="2" r:id="rId3"/>
+    <sheet name="UV-WMS Admin April" sheetId="3" r:id="rId4"/>
+    <sheet name="UV-WMS Admin May" sheetId="4" r:id="rId5"/>
+    <sheet name="UV-WMS Admin June" sheetId="5" r:id="rId6"/>
+    <sheet name="UV-WMS Admin July" sheetId="6" r:id="rId7"/>
+    <sheet name="UV-WMS Admin August" sheetId="7" r:id="rId8"/>
+    <sheet name="UV-WMS Admin September" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -871,12 +872,767 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27991520-C614-4BFB-ADD8-628FF075C04B}">
+  <dimension ref="A1:AJ15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>45658</v>
+      </c>
+      <c r="G1" s="1">
+        <v>45659</v>
+      </c>
+      <c r="H1" s="1">
+        <v>45660</v>
+      </c>
+      <c r="I1" s="1">
+        <v>45661</v>
+      </c>
+      <c r="J1" s="1">
+        <v>45662</v>
+      </c>
+      <c r="K1" s="1">
+        <v>45663</v>
+      </c>
+      <c r="L1" s="1">
+        <v>45664</v>
+      </c>
+      <c r="M1" s="1">
+        <v>45665</v>
+      </c>
+      <c r="N1" s="1">
+        <v>45666</v>
+      </c>
+      <c r="O1" s="1">
+        <v>45667</v>
+      </c>
+      <c r="P1" s="1">
+        <v>45668</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>45669</v>
+      </c>
+      <c r="R1" s="1">
+        <v>45670</v>
+      </c>
+      <c r="S1" s="1">
+        <v>45671</v>
+      </c>
+      <c r="T1" s="1">
+        <v>45672</v>
+      </c>
+      <c r="U1" s="1">
+        <v>45673</v>
+      </c>
+      <c r="V1" s="1">
+        <v>45674</v>
+      </c>
+      <c r="W1" s="1">
+        <v>45675</v>
+      </c>
+      <c r="X1" s="1">
+        <v>45676</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>45677</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>45678</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>45679</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>45680</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>45681</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>45682</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>45683</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>45684</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>45685</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>45686</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>45687</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>45688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>35898</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2">
+        <v>33548</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="7"/>
+      <c r="O4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44429</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="7"/>
+      <c r="O5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
+        <v>36698</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ6" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45078</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2">
+        <f>COUNTIF(F3:AI3,"WFO")</f>
+        <v>7</v>
+      </c>
+      <c r="C11" s="2">
+        <f>COUNTIF(F4:AI4,"WFH")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2">
+        <f>COUNTIF(F4:AI4,"WFO")</f>
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
+        <f>COUNTIF(F5:AI5,"WFH")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2">
+        <f>COUNTIF(F5:AI5,"WFO")</f>
+        <v>7</v>
+      </c>
+      <c r="C13" s="2">
+        <f>COUNTIF(F6:AI6,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2">
+        <f>COUNTIF(F6:AI6,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <f>COUNTIF(F7:AI7,"WFH")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2">
+        <f>COUNTIF(F7:AI7,"WFO")</f>
+        <v>8</v>
+      </c>
+      <c r="C15" s="2" t="e">
+        <f>COUNTIF(#REF!,"WFH")</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A6D4258-8D1D-40C7-BB83-4C4F9F65CC0B}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="T28" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,7 +2319,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E625ADA5-2D1E-431C-8817-0E3A7680EE75}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AJ15"/>
@@ -2381,7 +3137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D25C68-D147-4871-A2A8-2CD748E8464B}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AI16"/>
@@ -3206,7 +3962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460154BA-7A2B-4633-BD09-4305E2926D5D}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AJ16"/>
@@ -4047,7 +4803,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B0C082-0457-4696-978D-1BE2DD3075D3}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
@@ -4850,7 +5606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D2793F-73F1-4265-B1CF-8D693D22CC02}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
@@ -5685,12 +6441,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F16C68-A443-46CF-B7FA-2968469C0FB5}">
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S14" sqref="A1:XFD1048576"/>
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6503,12 +7259,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7CEAED-F464-426C-A766-484A87191C7F}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6745,10 +7501,18 @@
       <c r="F3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="2"/>
@@ -6794,9 +7558,15 @@
       <c r="F4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="J4" s="6" t="s">
         <v>24</v>
       </c>
@@ -6849,10 +7619,18 @@
       <c r="F5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="G5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="2"/>
@@ -6898,10 +7676,18 @@
       <c r="F6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="G6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="2"/>
@@ -6947,10 +7733,18 @@
       <c r="F7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="G7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="2"/>
@@ -7031,11 +7825,11 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -7044,11 +7838,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -7057,11 +7851,11 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -7074,7 +7868,7 @@
       </c>
       <c r="C16" s="2">
         <f>COUNTIF(F6:AI6,"WFH")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7083,11 +7877,11 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-05
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3759E6B-AEDC-4F54-83A0-37B0CB3338DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7326BF-F16D-480B-A5B0-BB8405EBC17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -879,29 +879,29 @@
       <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>45688</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1111,7 +1111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1635,30 +1635,30 @@
       <selection activeCell="T28" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1850,7 +1850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -2329,28 +2329,28 @@
       <selection pane="topRight" activeCell="AC6" sqref="AC6:AG6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>45747</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2560,7 +2560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2738,7 +2738,7 @@
       <c r="AI4" s="2"/>
       <c r="AJ4" s="13"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2826,7 +2826,7 @@
       <c r="AI5" s="2"/>
       <c r="AJ5" s="13"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2914,7 +2914,7 @@
       <c r="AI6" s="2"/>
       <c r="AJ6" s="13"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3002,7 +3002,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="13"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3040,7 +3040,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="14"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -3147,29 +3147,29 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3373,7 +3373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3828,7 +3828,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3865,7 +3865,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -3972,29 +3972,29 @@
       <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>45808</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4204,7 +4204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -4296,7 +4296,7 @@
       </c>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -4480,7 +4480,7 @@
       </c>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -4572,7 +4572,7 @@
       </c>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -4664,7 +4664,7 @@
       </c>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -4701,7 +4701,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -4812,15 +4812,15 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4927,7 +4927,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5024,7 +5024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -5506,7 +5506,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -5556,7 +5556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -5614,17 +5614,17 @@
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>45869</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5834,7 +5834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6341,7 +6341,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -6449,18 +6449,18 @@
       <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -6571,7 +6571,7 @@
       </c>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -6671,7 +6671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -6761,7 +6761,7 @@
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -6851,7 +6851,7 @@
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -6941,7 +6941,7 @@
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -7031,7 +7031,7 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -7121,7 +7121,7 @@
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -7159,7 +7159,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -7183,7 +7183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -7209,7 +7209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -7263,22 +7263,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7CEAED-F464-426C-A766-484A87191C7F}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -7385,7 +7385,7 @@
         <v>45930</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -7482,7 +7482,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -7539,7 +7539,7 @@
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -7572,9 +7572,15 @@
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="M4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="P4" s="6" t="s">
         <v>24</v>
       </c>
@@ -7600,7 +7606,7 @@
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -7657,7 +7663,7 @@
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -7714,7 +7720,7 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -7771,7 +7777,7 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -7808,7 +7814,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -7819,7 +7825,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -7832,7 +7838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -7842,10 +7848,10 @@
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -7858,7 +7864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -7871,7 +7877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-08
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7326BF-F16D-480B-A5B0-BB8405EBC17E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9C7F5F-538C-405C-B935-89360DCED813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27991520-C614-4BFB-ADD8-628FF075C04B}">
   <dimension ref="A1:AJ15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -899,6 +899,8 @@
     <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.35">
@@ -1127,61 +1129,73 @@
       <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="F3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
       <c r="R3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG3" s="5" t="s">
-        <v>17</v>
+      <c r="T3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="AH3" s="4" t="s">
         <v>16</v>
@@ -1209,63 +1223,73 @@
       <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="F4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
       <c r="K4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG4" s="5" t="s">
-        <v>17</v>
+      <c r="M4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="AH4" s="4" t="s">
         <v>16</v>
@@ -1293,63 +1317,73 @@
       <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="F5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
       <c r="K5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="7"/>
-      <c r="O5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="L5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
       <c r="R5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
-      <c r="AF5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG5" s="5" t="s">
-        <v>17</v>
+      <c r="S5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG5" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="AH5" s="4" t="s">
         <v>16</v>
@@ -1377,82 +1411,82 @@
       <c r="E6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="X6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AG6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>24</v>
+      <c r="F6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ6" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.35">
@@ -1471,61 +1505,73 @@
       <c r="E7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="F7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
       <c r="K7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="L7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
       <c r="R7" s="4" t="s">
         <v>16</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG7" s="5" t="s">
-        <v>17</v>
+      <c r="T7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="AH7" s="4" t="s">
         <v>16</v>
@@ -1554,11 +1600,11 @@
       </c>
       <c r="B11" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.35">
@@ -1567,7 +1613,7 @@
       </c>
       <c r="B12" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -1580,11 +1626,11 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F6:AI6,"WFH")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.35">
@@ -1593,11 +1639,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F6:AI6,"WFO")</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.35">
@@ -1606,7 +1652,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2" t="e">
         <f>COUNTIF(#REF!,"WFH")</f>
@@ -1631,8 +1677,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T28" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC7" sqref="AC7:AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1902,9 +1948,15 @@
       </c>
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
+      <c r="V3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Y3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1913,9 +1965,15 @@
       </c>
       <c r="AA3" s="7"/>
       <c r="AB3" s="7"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
+      <c r="AC3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AF3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1977,9 +2035,15 @@
       </c>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
+      <c r="V4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Y4" s="5" t="s">
         <v>17</v>
       </c>
@@ -1988,9 +2052,15 @@
       </c>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
+      <c r="AC4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AF4" s="5" t="s">
         <v>17</v>
       </c>
@@ -2052,9 +2122,15 @@
       </c>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
+      <c r="V5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Y5" s="5" t="s">
         <v>17</v>
       </c>
@@ -2063,9 +2139,15 @@
       </c>
       <c r="AA5" s="7"/>
       <c r="AB5" s="7"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
-      <c r="AE5" s="2"/>
+      <c r="AC5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AF5" s="5" t="s">
         <v>17</v>
       </c>
@@ -2210,9 +2292,15 @@
       </c>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
+      <c r="V7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Y7" s="5" t="s">
         <v>17</v>
       </c>
@@ -2221,9 +2309,15 @@
       </c>
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
+      <c r="AC7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AF7" s="5" t="s">
         <v>17</v>
       </c>
@@ -2248,7 +2342,7 @@
       </c>
       <c r="B11" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -2261,7 +2355,7 @@
       </c>
       <c r="B12" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -2274,7 +2368,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F6:AI6,"WFH")</f>
@@ -2300,7 +2394,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2" t="e">
         <f>COUNTIF(#REF!,"WFH")</f>
@@ -6445,8 +6539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F16C68-A443-46CF-B7FA-2968469C0FB5}">
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7263,8 +7357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7CEAED-F464-426C-A766-484A87191C7F}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:O4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7515,7 +7609,9 @@
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
-      <c r="M3" s="2"/>
+      <c r="M3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -7639,7 +7735,9 @@
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
-      <c r="M5" s="2"/>
+      <c r="M5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
@@ -7696,7 +7794,9 @@
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-      <c r="M6" s="2"/>
+      <c r="M6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -7753,7 +7853,9 @@
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="2"/>
+      <c r="M7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
@@ -7831,7 +7933,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
@@ -7857,7 +7959,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -7883,7 +7985,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-10
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9C7F5F-538C-405C-B935-89360DCED813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017F7DBE-FF5A-4E9E-ABF0-8E0AC0E6FC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27991520-C614-4BFB-ADD8-628FF075C04B}">
   <dimension ref="A1:AJ15"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1616,7 +1616,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="2">
-        <f>COUNTIF(F5:AI5,"WFH")</f>
+        <f t="shared" ref="C12:C15" si="0">COUNTIF(F5:AI5,"WFH")</f>
         <v>9</v>
       </c>
     </row>
@@ -1629,7 +1629,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="2">
-        <f>COUNTIF(F6:AI6,"WFH")</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="2">
-        <f>COUNTIF(F7:AI7,"WFH")</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -1654,9 +1654,9 @@
         <f>COUNTIF(F7:AI7,"WFO")</f>
         <v>12</v>
       </c>
-      <c r="C15" s="2" t="e">
-        <f>COUNTIF(#REF!,"WFH")</f>
-        <v>#REF!</v>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1677,8 +1677,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC7" sqref="AC7:AE7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2371,7 +2371,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="2">
-        <f>COUNTIF(F6:AI6,"WFH")</f>
+        <f t="shared" ref="C13:C15" si="0">COUNTIF(F6:AI6,"WFH")</f>
         <v>0</v>
       </c>
     </row>
@@ -2384,7 +2384,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="2">
-        <f>COUNTIF(F7:AI7,"WFH")</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -2396,9 +2396,9 @@
         <f>COUNTIF(F7:AI7,"WFO")</f>
         <v>13</v>
       </c>
-      <c r="C15" s="2" t="e">
-        <f>COUNTIF(#REF!,"WFH")</f>
-        <v>#REF!</v>
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7357,8 +7357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7CEAED-F464-426C-A766-484A87191C7F}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7612,8 +7612,12 @@
       <c r="M3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="N3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="7"/>
@@ -7738,8 +7742,12 @@
       <c r="M5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="N5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="7"/>
@@ -7797,10 +7805,18 @@
       <c r="M6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
+      <c r="N6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
       <c r="T6" s="2"/>
@@ -7856,8 +7872,12 @@
       <c r="M7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="N7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="7"/>
@@ -7933,7 +7953,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
@@ -7959,7 +7979,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -7985,7 +8005,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-11
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017F7DBE-FF5A-4E9E-ABF0-8E0AC0E6FC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13275858-792D-4813-BB10-5D3952C6874C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -7358,7 +7358,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="P7" sqref="P7:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7618,8 +7618,12 @@
       <c r="O3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="P3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="T3" s="2"/>
@@ -7748,8 +7752,12 @@
       <c r="O5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
+      <c r="P5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="2"/>
@@ -7878,8 +7886,12 @@
       <c r="O7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
+      <c r="P7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
       <c r="T7" s="2"/>
@@ -7957,7 +7969,7 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.35">
@@ -7983,7 +7995,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.35">
@@ -8009,7 +8021,7 @@
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-15
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13275858-792D-4813-BB10-5D3952C6874C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94643F8-7492-431B-93FB-2FBC4F7FAAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -879,31 +879,31 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>45688</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1113,7 +1113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1681,30 +1681,30 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1896,7 +1896,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -2423,28 +2423,28 @@
       <selection pane="topRight" activeCell="AC6" sqref="AC6:AG6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>45747</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2654,7 +2654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2832,7 +2832,7 @@
       <c r="AI4" s="2"/>
       <c r="AJ4" s="13"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2920,7 +2920,7 @@
       <c r="AI5" s="2"/>
       <c r="AJ5" s="13"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -3008,7 +3008,7 @@
       <c r="AI6" s="2"/>
       <c r="AJ6" s="13"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3096,7 +3096,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="13"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3134,7 +3134,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="14"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -3241,29 +3241,29 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3467,7 +3467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3959,7 +3959,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -4066,29 +4066,29 @@
       <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>45808</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4298,7 +4298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -4390,7 +4390,7 @@
       </c>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -4482,7 +4482,7 @@
       </c>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -4574,7 +4574,7 @@
       </c>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -4795,7 +4795,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -4906,15 +4906,15 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5118,7 +5118,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5296,7 +5296,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5385,7 +5385,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -5600,7 +5600,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -5624,7 +5624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -5708,17 +5708,17 @@
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>45869</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5928,7 +5928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6435,7 +6435,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -6446,7 +6446,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -6459,7 +6459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -6472,7 +6472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -6498,7 +6498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -6543,18 +6543,18 @@
       <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -6665,7 +6665,7 @@
       </c>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -6765,7 +6765,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -6855,7 +6855,7 @@
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -6945,7 +6945,7 @@
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -7035,7 +7035,7 @@
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -7125,7 +7125,7 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -7215,7 +7215,7 @@
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -7253,7 +7253,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -7264,7 +7264,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -7277,7 +7277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -7303,7 +7303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -7358,21 +7358,21 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7:Q7"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -7479,7 +7479,7 @@
         <v>45930</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -7576,7 +7576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -7626,7 +7626,9 @@
       </c>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
-      <c r="T3" s="2"/>
+      <c r="T3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
@@ -7643,7 +7645,7 @@
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -7693,7 +7695,9 @@
       </c>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
-      <c r="T4" s="2"/>
+      <c r="T4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
@@ -7710,7 +7714,7 @@
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -7760,7 +7764,9 @@
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
-      <c r="T5" s="2"/>
+      <c r="T5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
@@ -7777,7 +7783,7 @@
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -7827,7 +7833,9 @@
       </c>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
-      <c r="T6" s="2"/>
+      <c r="T6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
@@ -7844,7 +7852,7 @@
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -7894,7 +7902,9 @@
       </c>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
-      <c r="T7" s="2"/>
+      <c r="T7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
@@ -7911,7 +7921,7 @@
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -7948,7 +7958,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -7959,46 +7969,46 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -8011,7 +8021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -8021,7 +8031,7 @@
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-16
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55835520-4429-48AC-9A28-785AF3DF695D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058CF8D3-B5D1-4BA9-82BB-A5093D6A863E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -7358,7 +7358,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7629,7 +7629,9 @@
       <c r="T3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="2"/>
+      <c r="U3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
@@ -7698,7 +7700,9 @@
       <c r="T4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="2"/>
+      <c r="U4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
@@ -7767,7 +7771,9 @@
       <c r="T5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="U5" s="2"/>
+      <c r="U5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
@@ -7836,7 +7842,9 @@
       <c r="T6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="U6" s="2"/>
+      <c r="U6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
@@ -7905,7 +7913,9 @@
       <c r="T7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="U7" s="2"/>
+      <c r="U7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
@@ -7975,7 +7985,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
@@ -7988,7 +7998,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -8001,7 +8011,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -8027,7 +8037,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-18
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F99CD97-C56D-4025-BEC6-416EBD65D74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE88AE36-8166-45A8-B49F-F40F1729F826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -7357,8 +7357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7CEAED-F464-426C-A766-484A87191C7F}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7632,9 +7632,15 @@
       <c r="U3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
+      <c r="V3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="2"/>
@@ -7703,9 +7709,15 @@
       <c r="U4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
+      <c r="V4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
       <c r="AA4" s="2"/>
@@ -7774,9 +7786,15 @@
       <c r="U5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
+      <c r="V5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
       <c r="AA5" s="2"/>
@@ -7845,9 +7863,15 @@
       <c r="U6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
+      <c r="V6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
       <c r="AA6" s="2"/>
@@ -7916,9 +7940,15 @@
       <c r="U7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
+      <c r="V7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
       <c r="AA7" s="2"/>
@@ -7985,11 +8015,11 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -7998,11 +8028,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -8011,7 +8041,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -8037,7 +8067,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-22
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE88AE36-8166-45A8-B49F-F40F1729F826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFD1B73-DD75-41E9-AD09-8DF849C7439E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -7357,8 +7357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7CEAED-F464-426C-A766-484A87191C7F}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7643,8 +7643,12 @@
       </c>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
+      <c r="AA3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
@@ -7720,7 +7724,9 @@
       </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
-      <c r="AA4" s="2"/>
+      <c r="AA4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
@@ -7792,12 +7798,14 @@
       <c r="W5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="X5" s="4" t="s">
-        <v>16</v>
+      <c r="X5" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
-      <c r="AA5" s="2"/>
+      <c r="AA5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
@@ -7874,7 +7882,9 @@
       </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
-      <c r="AA6" s="2"/>
+      <c r="AA6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
@@ -7940,18 +7950,20 @@
       <c r="U7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="V7" s="4" t="s">
-        <v>16</v>
+      <c r="V7" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="W7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="X7" s="4" t="s">
-        <v>16</v>
+      <c r="X7" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
-      <c r="AA7" s="2"/>
+      <c r="AA7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
@@ -8028,7 +8040,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -8045,7 +8057,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -8067,11 +8079,11 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-23
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFD1B73-DD75-41E9-AD09-8DF849C7439E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7D687B-8626-434E-8C4F-4098EDA95C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -7358,7 +7358,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+      <selection activeCell="AE15" sqref="AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7370,6 +7370,7 @@
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
@@ -7727,7 +7728,9 @@
       <c r="AA4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AB4" s="2"/>
+      <c r="AB4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
@@ -7806,7 +7809,9 @@
       <c r="AA5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AB5" s="2"/>
+      <c r="AB5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
@@ -7885,7 +7890,9 @@
       <c r="AA6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AB6" s="2"/>
+      <c r="AB6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
@@ -7964,7 +7971,9 @@
       <c r="AA7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AB7" s="2"/>
+      <c r="AB7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
@@ -8040,7 +8049,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -8053,7 +8062,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -8079,7 +8088,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-24
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7D687B-8626-434E-8C4F-4098EDA95C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2053974-4271-4FAE-A309-71AF0CE0627D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -7358,7 +7358,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AE15" sqref="AE15"/>
+      <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7650,7 +7650,9 @@
       <c r="AB3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AC3" s="2"/>
+      <c r="AC3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="7"/>
@@ -7731,7 +7733,9 @@
       <c r="AB4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AC4" s="2"/>
+      <c r="AC4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
       <c r="AF4" s="7"/>
@@ -7812,7 +7816,9 @@
       <c r="AB5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AC5" s="2"/>
+      <c r="AC5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="7"/>
@@ -7893,7 +7899,9 @@
       <c r="AB6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AC6" s="2"/>
+      <c r="AC6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
       <c r="AF6" s="7"/>
@@ -7974,7 +7982,9 @@
       <c r="AB7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AC7" s="2"/>
+      <c r="AC7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="7"/>
@@ -8036,7 +8046,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
@@ -8049,7 +8059,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -8062,7 +8072,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -8088,7 +8098,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-25
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2053974-4271-4FAE-A309-71AF0CE0627D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D50705-B007-4058-B47E-F0FD5BD47E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -7358,7 +7358,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AC7" sqref="AC7"/>
+      <selection activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7653,7 +7653,9 @@
       <c r="AC3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AD3" s="2"/>
+      <c r="AD3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AE3" s="2"/>
       <c r="AF3" s="7"/>
       <c r="AG3" s="7"/>
@@ -7736,7 +7738,9 @@
       <c r="AC4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="2"/>
+      <c r="AD4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AE4" s="2"/>
       <c r="AF4" s="7"/>
       <c r="AG4" s="7"/>
@@ -7819,7 +7823,9 @@
       <c r="AC5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AD5" s="2"/>
+      <c r="AD5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AE5" s="2"/>
       <c r="AF5" s="7"/>
       <c r="AG5" s="7"/>
@@ -7902,7 +7908,9 @@
       <c r="AC6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AD6" s="2"/>
+      <c r="AD6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AE6" s="2"/>
       <c r="AF6" s="7"/>
       <c r="AG6" s="7"/>
@@ -7985,7 +7993,9 @@
       <c r="AC7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AD7" s="2"/>
+      <c r="AD7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AE7" s="2"/>
       <c r="AF7" s="7"/>
       <c r="AG7" s="7"/>
@@ -8050,7 +8060,7 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -8063,7 +8073,7 @@
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -8076,7 +8086,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -8102,7 +8112,7 @@
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-09-29
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9614DA21-1B4E-4FD0-A8E8-3179FF128D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F76101D-626D-4AB5-B0E4-FCCCEA079EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -7357,8 +7357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7CEAED-F464-426C-A766-484A87191C7F}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="AB5" sqref="AB5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AH3" sqref="AH3:AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7656,10 +7656,14 @@
       <c r="AD3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE3" s="2"/>
+      <c r="AE3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AF3" s="7"/>
       <c r="AG3" s="7"/>
-      <c r="AH3" s="2"/>
+      <c r="AH3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AI3" s="2"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -7741,10 +7745,14 @@
       <c r="AD4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE4" s="2"/>
+      <c r="AE4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AF4" s="7"/>
       <c r="AG4" s="7"/>
-      <c r="AH4" s="2"/>
+      <c r="AH4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AI4" s="2"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -7826,10 +7834,14 @@
       <c r="AD5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE5" s="2"/>
+      <c r="AE5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AF5" s="7"/>
       <c r="AG5" s="7"/>
-      <c r="AH5" s="2"/>
+      <c r="AH5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AI5" s="2"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
@@ -7911,10 +7923,14 @@
       <c r="AD6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AE6" s="2"/>
+      <c r="AE6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AF6" s="7"/>
       <c r="AG6" s="7"/>
-      <c r="AH6" s="2"/>
+      <c r="AH6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AI6" s="2"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
@@ -7996,10 +8012,14 @@
       <c r="AD7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE7" s="2"/>
+      <c r="AE7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AF7" s="7"/>
       <c r="AG7" s="7"/>
-      <c r="AH7" s="2"/>
+      <c r="AH7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AI7" s="2"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
@@ -8056,11 +8076,11 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -8069,11 +8089,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -8082,11 +8102,11 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -8108,11 +8128,11 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-10-01
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F76101D-626D-4AB5-B0E4-FCCCEA079EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D757A90E-7A7E-4228-9F29-6F0317CD0B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -22,6 +22,7 @@
     <sheet name="UV-WMS Admin July" sheetId="6" r:id="rId7"/>
     <sheet name="UV-WMS Admin August" sheetId="7" r:id="rId8"/>
     <sheet name="UV-WMS Admin September" sheetId="8" r:id="rId9"/>
+    <sheet name="UV-WMS Admin October" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -352,7 +353,37 @@
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1672,6 +1703,637 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{826FC1B3-53E6-4D35-9223-A0DEC05CDA48}">
+  <dimension ref="A1:AJ17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>45931</v>
+      </c>
+      <c r="G1" s="1">
+        <v>45932</v>
+      </c>
+      <c r="H1" s="1">
+        <v>45933</v>
+      </c>
+      <c r="I1" s="1">
+        <v>45934</v>
+      </c>
+      <c r="J1" s="1">
+        <v>45935</v>
+      </c>
+      <c r="K1" s="1">
+        <v>45936</v>
+      </c>
+      <c r="L1" s="1">
+        <v>45937</v>
+      </c>
+      <c r="M1" s="1">
+        <v>45938</v>
+      </c>
+      <c r="N1" s="1">
+        <v>45939</v>
+      </c>
+      <c r="O1" s="1">
+        <v>45940</v>
+      </c>
+      <c r="P1" s="1">
+        <v>45941</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>45942</v>
+      </c>
+      <c r="R1" s="1">
+        <v>45943</v>
+      </c>
+      <c r="S1" s="1">
+        <v>45944</v>
+      </c>
+      <c r="T1" s="1">
+        <v>45945</v>
+      </c>
+      <c r="U1" s="1">
+        <v>45946</v>
+      </c>
+      <c r="V1" s="1">
+        <v>45947</v>
+      </c>
+      <c r="W1" s="1">
+        <v>45948</v>
+      </c>
+      <c r="X1" s="1">
+        <v>45949</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>45950</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>45951</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>45952</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>45953</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>45954</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>45955</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>45956</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>45957</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>45958</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>45959</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>45960</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>45961</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>35898</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2">
+        <v>33548</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44429</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
+        <v>36698</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45078</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <f>COUNTIF(F3:AI3,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <f>COUNTIF(F3:AI3,"WFH")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <f>COUNTIF(F4:AI4,"WFO")</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <f>COUNTIF(F4:AI4,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2">
+        <f>COUNTIF(F5:AI5,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <f>COUNTIF(F5:AI5,"WFH")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2">
+        <f>COUNTIF(F6:AI6,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <f>COUNTIF(F6:AI6,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2">
+        <f>COUNTIF(F7:AI7,"WFO")</f>
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <f>COUNTIF(F7:AI7,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="B13:B17">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A6D4258-8D1D-40C7-BB83-4C4F9F65CC0B}">
   <sheetPr codeName="Sheet1"/>
@@ -3220,10 +3882,10 @@
     <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:B15">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4045,10 +4707,10 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4881,15 +5543,15 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="2" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="lessThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5686,13 +6348,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6521,13 +7183,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6540,7 +7202,7 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7339,13 +8001,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7358,7 +8020,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3:AH7"/>
+      <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7664,7 +8326,9 @@
       <c r="AH3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="2"/>
+      <c r="AI3" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -7753,7 +8417,9 @@
       <c r="AH4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AI4" s="2"/>
+      <c r="AI4" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -7842,7 +8508,9 @@
       <c r="AH5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AI5" s="2"/>
+      <c r="AI5" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -7931,7 +8599,9 @@
       <c r="AH6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AI6" s="2"/>
+      <c r="AI6" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -8020,7 +8690,9 @@
       <c r="AH7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AI7" s="2"/>
+      <c r="AI7" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -8076,7 +8748,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
@@ -8089,7 +8761,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -8106,7 +8778,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -8128,7 +8800,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
@@ -8145,13 +8817,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Daily attendance update - 2025-10-06
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC404B3-BC9B-4460-A4CB-C4B89B7B9BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5E1F23-43F0-46D7-B795-DDB363A3F467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -1708,7 +1708,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1958,10 +1958,14 @@
       <c r="G3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="2"/>
+      <c r="K3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -2010,10 +2014,14 @@
       <c r="G4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="2"/>
+      <c r="K4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -2067,7 +2075,9 @@
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="2"/>
+      <c r="K5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -2116,10 +2126,14 @@
       <c r="G6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="2"/>
+      <c r="K6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -2168,10 +2182,14 @@
       <c r="G7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="2"/>
+      <c r="K7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -2253,11 +2271,11 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -2266,11 +2284,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -2279,7 +2297,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -2305,7 +2323,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-10-08
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95289BB1-744F-4B02-B78C-4EB84667E971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916B2AEE-5360-462D-925B-E9BAE22E961B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="UV-WMS Admin August" sheetId="7" r:id="rId8"/>
     <sheet name="UV-WMS Admin September" sheetId="8" r:id="rId9"/>
     <sheet name="UV-WMS Admin October" sheetId="10" r:id="rId10"/>
+    <sheet name="UV-WMS Admin November" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -353,7 +354,37 @@
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -910,31 +941,31 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1044,7 +1075,7 @@
         <v>45688</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1144,7 +1175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1238,7 +1269,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1332,7 +1363,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1426,7 +1457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1520,7 +1551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1614,7 +1645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -1625,7 +1656,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1638,7 +1669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1651,7 +1682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1664,7 +1695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1677,7 +1708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1707,26 +1738,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{826FC1B3-53E6-4D35-9223-A0DEC05CDA48}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="33" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1836,7 +1875,7 @@
         <v>45961</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1936,7 +1975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1966,8 +2005,12 @@
       <c r="K3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="L3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="7"/>
@@ -1976,10 +2019,14 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
+      <c r="V3" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="W3" s="7"/>
       <c r="X3" s="7"/>
-      <c r="Y3" s="2"/>
+      <c r="Y3" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
@@ -1992,7 +2039,7 @@
       <c r="AI3" s="2"/>
       <c r="AJ3" s="2"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2022,8 +2069,12 @@
       <c r="K4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="L4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="7"/>
@@ -2035,8 +2086,12 @@
       <c r="V4" s="2"/>
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
+      <c r="Y4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
@@ -2048,7 +2103,7 @@
       <c r="AI4" s="2"/>
       <c r="AJ4" s="2"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2078,8 +2133,12 @@
       <c r="K5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="L5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="7"/>
@@ -2091,7 +2150,9 @@
       <c r="V5" s="2"/>
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
-      <c r="Y5" s="2"/>
+      <c r="Y5" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
@@ -2104,7 +2165,7 @@
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2134,8 +2195,12 @@
       <c r="K6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="L6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="7"/>
@@ -2147,7 +2212,9 @@
       <c r="V6" s="2"/>
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
-      <c r="Y6" s="2"/>
+      <c r="Y6" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
@@ -2160,7 +2227,7 @@
       <c r="AI6" s="2"/>
       <c r="AJ6" s="2"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2190,8 +2257,12 @@
       <c r="K7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="L7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="7"/>
@@ -2203,7 +2274,9 @@
       <c r="V7" s="2"/>
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
-      <c r="Y7" s="2"/>
+      <c r="Y7" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
@@ -2216,7 +2289,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2254,7 +2327,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -2265,33 +2338,642 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2">
+        <f>COUNTIF(F5:AI5,"WFO")</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <f>COUNTIF(F5:AI5,"WFH")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2">
+        <f>COUNTIF(F6:AI6,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <f>COUNTIF(F6:AI6,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2">
+        <f>COUNTIF(F7:AI7,"WFO")</f>
+        <v>5</v>
+      </c>
+      <c r="C17" s="2">
+        <f>COUNTIF(F7:AI7,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="B13:B17">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42BC0F2-E7C0-48B4-8AB8-C4D08FDA0656}">
+  <dimension ref="A1:AI17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>45962</v>
+      </c>
+      <c r="G1" s="1">
+        <v>45963</v>
+      </c>
+      <c r="H1" s="1">
+        <v>45964</v>
+      </c>
+      <c r="I1" s="1">
+        <v>45965</v>
+      </c>
+      <c r="J1" s="1">
+        <v>45966</v>
+      </c>
+      <c r="K1" s="1">
+        <v>45967</v>
+      </c>
+      <c r="L1" s="1">
+        <v>45968</v>
+      </c>
+      <c r="M1" s="1">
+        <v>45969</v>
+      </c>
+      <c r="N1" s="1">
+        <v>45970</v>
+      </c>
+      <c r="O1" s="1">
+        <v>45971</v>
+      </c>
+      <c r="P1" s="1">
+        <v>45972</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>45973</v>
+      </c>
+      <c r="R1" s="1">
+        <v>45974</v>
+      </c>
+      <c r="S1" s="1">
+        <v>45975</v>
+      </c>
+      <c r="T1" s="1">
+        <v>45976</v>
+      </c>
+      <c r="U1" s="1">
+        <v>45977</v>
+      </c>
+      <c r="V1" s="1">
+        <v>45978</v>
+      </c>
+      <c r="W1" s="1">
+        <v>45979</v>
+      </c>
+      <c r="X1" s="1">
+        <v>45980</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>45981</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>45982</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>45983</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>45984</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>45985</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>45986</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>45987</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>45988</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>45989</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>45990</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>45991</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>35898</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2">
+        <v>33548</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="7"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44429</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
+        <v>36698</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45078</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <f>COUNTIF(F3:AI3,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <f>COUNTIF(F3:AI3,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <f>COUNTIF(F4:AI4,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <f>COUNTIF(F4:AI4,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -2301,10 +2983,10 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -2317,13 +2999,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
@@ -2363,30 +3045,30 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -2487,7 +3169,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2578,7 +3260,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2663,7 +3345,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2750,7 +3432,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2837,7 +3519,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2922,7 +3604,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3007,7 +3689,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -3018,7 +3700,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -3031,7 +3713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -3044,7 +3726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -3057,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -3070,7 +3752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -3105,28 +3787,28 @@
       <selection pane="topRight" activeCell="AC6" sqref="AC6:AG6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -3236,7 +3918,7 @@
         <v>45747</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3336,7 +4018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -3426,7 +4108,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -3514,7 +4196,7 @@
       <c r="AI4" s="2"/>
       <c r="AJ4" s="13"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3602,7 +4284,7 @@
       <c r="AI5" s="2"/>
       <c r="AJ5" s="13"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -3690,7 +4372,7 @@
       <c r="AI6" s="2"/>
       <c r="AJ6" s="13"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3778,7 +4460,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="13"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3816,7 +4498,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="14"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -3827,7 +4509,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -3840,7 +4522,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -3853,7 +4535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -3866,7 +4548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -3879,7 +4561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -3902,10 +4584,10 @@
     <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:B15">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3923,29 +4605,29 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4052,7 +4734,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4149,7 +4831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -4240,7 +4922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -4331,7 +5013,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -4422,7 +5104,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -4513,7 +5195,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -4604,7 +5286,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -4641,7 +5323,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -4652,7 +5334,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -4665,7 +5347,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -4678,7 +5360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -4691,7 +5373,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -4704,7 +5386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -4727,10 +5409,10 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4748,29 +5430,29 @@
       <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4880,7 +5562,7 @@
         <v>45808</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4980,7 +5662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5072,7 +5754,7 @@
       </c>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5164,7 +5846,7 @@
       </c>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5256,7 +5938,7 @@
       </c>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -5348,7 +6030,7 @@
       </c>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -5440,7 +6122,7 @@
       </c>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -5477,7 +6159,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -5488,7 +6170,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -5501,7 +6183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -5514,7 +6196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -5527,7 +6209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -5540,7 +6222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -5563,15 +6245,15 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="cellIs" dxfId="17" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="lessThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5588,15 +6270,15 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -5703,7 +6385,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5800,7 +6482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5889,7 +6571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5978,7 +6660,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -6067,7 +6749,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -6156,7 +6838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -6245,7 +6927,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6282,7 +6964,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
@@ -6293,7 +6975,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -6306,7 +6988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -6319,7 +7001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -6332,7 +7014,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -6345,7 +7027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -6368,13 +7050,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6390,17 +7072,17 @@
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -6510,7 +7192,7 @@
         <v>45869</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -6610,7 +7292,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -6704,7 +7386,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -6798,7 +7480,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -6892,7 +7574,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -6986,7 +7668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -7080,7 +7762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -7117,7 +7799,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -7128,7 +7810,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -7141,7 +7823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -7154,7 +7836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -7167,7 +7849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -7180,7 +7862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -7203,13 +7885,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7225,18 +7907,18 @@
       <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -7347,7 +8029,7 @@
       </c>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -7447,7 +8129,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -7537,7 +8219,7 @@
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -7627,7 +8309,7 @@
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -7717,7 +8399,7 @@
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -7807,7 +8489,7 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -7897,7 +8579,7 @@
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -7935,7 +8617,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -7946,7 +8628,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -7959,7 +8641,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -7972,7 +8654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -7985,7 +8667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -7998,7 +8680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -8021,13 +8703,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8043,19 +8725,19 @@
       <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -8162,7 +8844,7 @@
         <v>45930</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -8259,7 +8941,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -8350,7 +9032,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -8441,7 +9123,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -8532,7 +9214,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -8623,7 +9305,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -8714,7 +9396,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -8751,7 +9433,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -8762,7 +9444,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -8775,7 +9457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -8788,7 +9470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -8801,7 +9483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -8814,7 +9496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -8837,13 +9519,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Daily attendance update - 2025-10-09
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916B2AEE-5360-462D-925B-E9BAE22E961B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922A78B6-52AB-4910-91E0-1BE1A489BA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1710" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -941,31 +941,31 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>45688</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1175,7 +1175,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1739,33 +1739,33 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="19" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="28" max="33" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="33" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>45961</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -1975,7 +1975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2011,7 +2011,9 @@
       <c r="M3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="2"/>
+      <c r="N3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="O3" s="2"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
@@ -2039,7 +2041,7 @@
       <c r="AI3" s="2"/>
       <c r="AJ3" s="2"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2075,7 +2077,9 @@
       <c r="M4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="2"/>
+      <c r="N4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="O4" s="2"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
@@ -2103,7 +2107,7 @@
       <c r="AI4" s="2"/>
       <c r="AJ4" s="2"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2139,7 +2143,9 @@
       <c r="M5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="2"/>
+      <c r="N5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="O5" s="2"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
@@ -2165,7 +2171,7 @@
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2201,7 +2207,9 @@
       <c r="M6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="2"/>
+      <c r="N6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="O6" s="2"/>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
@@ -2227,7 +2235,7 @@
       <c r="AI6" s="2"/>
       <c r="AJ6" s="2"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2263,7 +2271,9 @@
       <c r="M7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="2"/>
+      <c r="N7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="O7" s="2"/>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
@@ -2277,10 +2287,18 @@
       <c r="Y7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
+      <c r="Z7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC7" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AD7" s="7"/>
       <c r="AE7" s="7"/>
       <c r="AF7" s="2"/>
@@ -2289,7 +2307,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2327,7 +2345,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -2338,7 +2356,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -2348,10 +2366,10 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -2361,23 +2379,23 @@
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -2390,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -2400,7 +2418,7 @@
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2432,29 +2450,29 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -2561,7 +2579,7 @@
         <v>45991</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -2658,7 +2676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2711,7 +2729,7 @@
       <c r="AH3" s="7"/>
       <c r="AI3" s="7"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -2758,7 +2776,7 @@
       <c r="AH4" s="7"/>
       <c r="AI4" s="7"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -2805,7 +2823,7 @@
       <c r="AH5" s="7"/>
       <c r="AI5" s="7"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2852,7 +2870,7 @@
       <c r="AH6" s="7"/>
       <c r="AI6" s="7"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2899,7 +2917,7 @@
       <c r="AH7" s="7"/>
       <c r="AI7" s="7"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2936,7 +2954,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -2947,7 +2965,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -2960,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -2973,7 +2991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -2986,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -2999,7 +3017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -3045,30 +3063,30 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -3169,7 +3187,7 @@
         <v>45716</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -3260,7 +3278,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -3345,7 +3363,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -3432,7 +3450,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3519,7 +3537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -3604,7 +3622,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -3689,7 +3707,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -3700,7 +3718,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -3713,7 +3731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -3726,7 +3744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -3739,7 +3757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -3752,7 +3770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -3787,28 +3805,28 @@
       <selection pane="topRight" activeCell="AC6" sqref="AC6:AG6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -3918,7 +3936,7 @@
         <v>45747</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4018,7 +4036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -4108,7 +4126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -4196,7 +4214,7 @@
       <c r="AI4" s="2"/>
       <c r="AJ4" s="13"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -4284,7 +4302,7 @@
       <c r="AI5" s="2"/>
       <c r="AJ5" s="13"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -4372,7 +4390,7 @@
       <c r="AI6" s="2"/>
       <c r="AJ6" s="13"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -4460,7 +4478,7 @@
       <c r="AI7" s="2"/>
       <c r="AJ7" s="13"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -4498,7 +4516,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="14"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -4509,7 +4527,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -4522,7 +4540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -4535,7 +4553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -4548,7 +4566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -4561,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -4605,29 +4623,29 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4734,7 +4752,7 @@
         <v>45777</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4831,7 +4849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -4922,7 +4940,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5013,7 +5031,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5104,7 +5122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -5195,7 +5213,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -5286,7 +5304,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -5323,7 +5341,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -5334,7 +5352,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -5347,7 +5365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -5360,7 +5378,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -5373,7 +5391,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -5386,7 +5404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -5430,29 +5448,29 @@
       <selection pane="topRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="32" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -5562,7 +5580,7 @@
         <v>45808</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -5662,7 +5680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5754,7 +5772,7 @@
       </c>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5846,7 +5864,7 @@
       </c>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -5938,7 +5956,7 @@
       </c>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -6030,7 +6048,7 @@
       </c>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -6122,7 +6140,7 @@
       </c>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6159,7 +6177,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -6170,7 +6188,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -6183,7 +6201,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -6196,7 +6214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -6209,7 +6227,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -6222,7 +6240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -6270,15 +6288,15 @@
       <selection pane="topRight" activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -6385,7 +6403,7 @@
         <v>45838</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -6482,7 +6500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -6571,7 +6589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -6660,7 +6678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -6749,7 +6767,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -6838,7 +6856,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -6927,7 +6945,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -6964,7 +6982,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
@@ -6975,7 +6993,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -6988,7 +7006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -7001,7 +7019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -7014,7 +7032,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -7027,7 +7045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -7072,17 +7090,17 @@
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -7192,7 +7210,7 @@
         <v>45869</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -7292,7 +7310,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -7386,7 +7404,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -7480,7 +7498,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -7574,7 +7592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -7668,7 +7686,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -7762,7 +7780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -7799,7 +7817,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -7810,7 +7828,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -7823,7 +7841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -7836,7 +7854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -7849,7 +7867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -7862,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -7907,18 +7925,18 @@
       <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -8029,7 +8047,7 @@
       </c>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -8129,7 +8147,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -8219,7 +8237,7 @@
       <c r="AI3" s="7"/>
       <c r="AJ3" s="7"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -8309,7 +8327,7 @@
       <c r="AI4" s="7"/>
       <c r="AJ4" s="7"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -8399,7 +8417,7 @@
       <c r="AI5" s="7"/>
       <c r="AJ5" s="7"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -8489,7 +8507,7 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -8579,7 +8597,7 @@
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -8617,7 +8635,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -8628,7 +8646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -8641,7 +8659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -8654,7 +8672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -8667,7 +8685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -8680,7 +8698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -8725,19 +8743,19 @@
       <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -8844,7 +8862,7 @@
         <v>45930</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -8941,7 +8959,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -9032,7 +9050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -9123,7 +9141,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -9214,7 +9232,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -9305,7 +9323,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -9396,7 +9414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -9433,7 +9451,7 @@
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>1</v>
       </c>
@@ -9444,7 +9462,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -9457,7 +9475,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -9470,7 +9488,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -9483,7 +9501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -9496,7 +9514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Daily attendance update - 2025-10-20
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922A78B6-52AB-4910-91E0-1BE1A489BA97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97D7F68-DD44-4370-BDFC-0C9E257DB6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -1738,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{826FC1B3-53E6-4D35-9223-A0DEC05CDA48}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2014,13 +2014,23 @@
       <c r="N3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="2"/>
+      <c r="O3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="R3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="V3" s="6" t="s">
         <v>24</v>
       </c>
@@ -2080,14 +2090,26 @@
       <c r="N4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="2"/>
+      <c r="O4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
+      <c r="R4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
       <c r="Y4" s="6" t="s">
@@ -2146,14 +2168,26 @@
       <c r="N5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="2"/>
+      <c r="O5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
+      <c r="R5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
       <c r="Y5" s="6" t="s">
@@ -2210,14 +2244,26 @@
       <c r="N6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="2"/>
+      <c r="O6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
+      <c r="R6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
       <c r="Y6" s="6" t="s">
@@ -2274,14 +2320,26 @@
       <c r="N7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="O7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
+      <c r="R7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
       <c r="Y7" s="6" t="s">
@@ -2362,11 +2420,11 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -2375,11 +2433,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -2388,11 +2446,11 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
@@ -2405,7 +2463,7 @@
       </c>
       <c r="C16" s="2">
         <f>COUNTIF(F6:AI6,"WFH")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2418,7 +2476,7 @@
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-10-21
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97D7F68-DD44-4370-BDFC-0C9E257DB6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C05C200-A12E-42D3-872A-DEB90804F8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1748" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -1739,7 +1739,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AH15" sqref="AH15"/>
+      <selection activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,7 +2039,9 @@
       <c r="Y3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z3" s="2"/>
+      <c r="Z3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
@@ -2193,7 +2195,9 @@
       <c r="Y5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="2"/>
+      <c r="Z5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
@@ -2261,18 +2265,26 @@
       <c r="U6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="V6" s="5" t="s">
-        <v>17</v>
+      <c r="V6" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
       <c r="Y6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
+      <c r="Z6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AD6" s="7"/>
       <c r="AE6" s="7"/>
       <c r="AF6" s="2"/>
@@ -2420,7 +2432,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
@@ -2446,7 +2458,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -2463,7 +2475,7 @@
       </c>
       <c r="C16" s="2">
         <f>COUNTIF(F6:AI6,"WFH")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Daily attendance update - 2025-10-23
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C05C200-A12E-42D3-872A-DEB90804F8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214CD60D-FFF8-4979-BAF0-2F0347A1E5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -1738,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{826FC1B3-53E6-4D35-9223-A0DEC05CDA48}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,8 +2042,12 @@
       <c r="Z3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
+      <c r="AA3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AC3" s="2"/>
       <c r="AD3" s="7"/>
       <c r="AE3" s="7"/>
@@ -2120,8 +2124,12 @@
       <c r="Z4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
+      <c r="AA4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AC4" s="2"/>
       <c r="AD4" s="7"/>
       <c r="AE4" s="7"/>
@@ -2198,8 +2206,12 @@
       <c r="Z5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
+      <c r="AA5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AC5" s="2"/>
       <c r="AD5" s="7"/>
       <c r="AE5" s="7"/>
@@ -2436,7 +2448,7 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -2445,7 +2457,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -2462,7 +2474,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Daily attendance update - 2025-10-28
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8601B6F8-CF82-4CE1-ACAA-E5D335EBFB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50A72FF-12EF-49DE-BA67-39DCDC8363C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1773" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -1738,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{826FC1B3-53E6-4D35-9223-A0DEC05CDA48}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="AA21" sqref="AA21"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,11 +2048,17 @@
       <c r="AB3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="2"/>
+      <c r="AC3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AD3" s="7"/>
       <c r="AE3" s="7"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
+      <c r="AF3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AH3" s="2"/>
       <c r="AI3" s="2"/>
       <c r="AJ3" s="2"/>
@@ -2130,11 +2136,17 @@
       <c r="AB4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AC4" s="2"/>
+      <c r="AC4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AD4" s="7"/>
       <c r="AE4" s="7"/>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
+      <c r="AF4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AH4" s="2"/>
       <c r="AI4" s="2"/>
       <c r="AJ4" s="2"/>
@@ -2212,11 +2224,17 @@
       <c r="AB5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AC5" s="2"/>
+      <c r="AC5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AD5" s="7"/>
       <c r="AE5" s="7"/>
-      <c r="AF5" s="2"/>
-      <c r="AG5" s="2"/>
+      <c r="AF5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
@@ -2299,8 +2317,12 @@
       </c>
       <c r="AD6" s="7"/>
       <c r="AE6" s="7"/>
-      <c r="AF6" s="2"/>
-      <c r="AG6" s="2"/>
+      <c r="AF6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AH6" s="2"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="2"/>
@@ -2383,8 +2405,12 @@
       </c>
       <c r="AD7" s="7"/>
       <c r="AE7" s="7"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
+      <c r="AF7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG7" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
@@ -2444,11 +2470,11 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -2457,11 +2483,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -2474,7 +2500,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
@@ -2487,7 +2513,7 @@
       </c>
       <c r="C16" s="2">
         <f>COUNTIF(F6:AI6,"WFH")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Daily attendance update - 2025-10-29
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50A72FF-12EF-49DE-BA67-39DCDC8363C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD181E8-E75B-4E3C-83CF-0F2D0E50FA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1773" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -1739,7 +1739,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3"/>
+      <selection activeCell="AH3" sqref="AH3:AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,7 +2059,9 @@
       <c r="AG3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AH3" s="2"/>
+      <c r="AH3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AI3" s="2"/>
       <c r="AJ3" s="2"/>
     </row>
@@ -2147,7 +2149,9 @@
       <c r="AG4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AH4" s="2"/>
+      <c r="AH4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AI4" s="2"/>
       <c r="AJ4" s="2"/>
     </row>
@@ -2235,7 +2239,9 @@
       <c r="AG5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AH5" s="2"/>
+      <c r="AH5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
     </row>
@@ -2323,7 +2329,9 @@
       <c r="AG6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AH6" s="2"/>
+      <c r="AH6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="2"/>
     </row>
@@ -2411,7 +2419,9 @@
       <c r="AG7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AH7" s="2"/>
+      <c r="AH7" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
     </row>
@@ -2470,7 +2480,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
@@ -2483,7 +2493,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -2500,7 +2510,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
@@ -2513,7 +2523,7 @@
       </c>
       <c r="C16" s="2">
         <f>COUNTIF(F6:AI6,"WFH")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Daily attendance update - 2025-11-03
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD181E8-E75B-4E3C-83CF-0F2D0E50FA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D8E5E5-6DCD-40D8-A280-28D8D7108A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -1738,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{826FC1B3-53E6-4D35-9223-A0DEC05CDA48}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AH3" sqref="AH3:AH7"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,8 +2062,12 @@
       <c r="AH3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AI3" s="2"/>
-      <c r="AJ3" s="2"/>
+      <c r="AI3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2152,8 +2156,12 @@
       <c r="AH4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AI4" s="2"/>
-      <c r="AJ4" s="2"/>
+      <c r="AI4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -2242,8 +2250,12 @@
       <c r="AH5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AI5" s="2"/>
-      <c r="AJ5" s="2"/>
+      <c r="AI5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ5" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -2332,8 +2344,12 @@
       <c r="AH6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AI6" s="2"/>
-      <c r="AJ6" s="2"/>
+      <c r="AI6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ6" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -2422,8 +2438,12 @@
       <c r="AH7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
+      <c r="AI7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ7" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -2484,7 +2504,7 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -2497,7 +2517,7 @@
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -2506,7 +2526,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -2523,7 +2543,7 @@
       </c>
       <c r="C16" s="2">
         <f>COUNTIF(F6:AI6,"WFH")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2567,8 +2587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42BC0F2-E7C0-48B4-8AB8-C4D08FDA0656}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2812,7 +2832,9 @@
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="2"/>
+      <c r="H3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -2865,7 +2887,9 @@
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -2912,7 +2936,9 @@
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="2"/>
+      <c r="H5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -2959,7 +2985,9 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="2"/>
+      <c r="H6" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -3006,7 +3034,9 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -3089,7 +3119,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
@@ -3115,7 +3145,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-11-07
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D8E5E5-6DCD-40D8-A280-28D8D7108A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A179D638-F615-4861-A065-265ADA29A0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -1739,7 +1739,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+      <selection activeCell="AA23" sqref="AA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2335,20 +2335,20 @@
       </c>
       <c r="AD6" s="7"/>
       <c r="AE6" s="7"/>
-      <c r="AF6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AI6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ6" s="5" t="s">
-        <v>17</v>
+      <c r="AF6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ6" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -2429,20 +2429,20 @@
       </c>
       <c r="AD7" s="7"/>
       <c r="AE7" s="7"/>
-      <c r="AF7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AG7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ7" s="6" t="s">
-        <v>24</v>
+      <c r="AF7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ7" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
@@ -2543,7 +2543,7 @@
       </c>
       <c r="C16" s="2">
         <f>COUNTIF(F6:AI6,"WFH")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2556,7 +2556,7 @@
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2588,7 +2588,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2832,13 +2832,21 @@
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="H3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="2"/>
@@ -2887,13 +2895,21 @@
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="2"/>
@@ -2939,10 +2955,18 @@
       <c r="H5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="I5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="2"/>
@@ -2986,12 +3010,20 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="2"/>
@@ -3035,12 +3067,20 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="2"/>
@@ -3119,11 +3159,11 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -3132,11 +3172,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -3145,11 +3185,11 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -3162,7 +3202,7 @@
       </c>
       <c r="C16" s="2">
         <f>COUNTIF(F6:AI6,"WFH")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3171,11 +3211,11 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-11-11
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC68073-85EE-483B-B6C0-C985F0916101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7C77A3-A7C1-4FF1-BA4C-619F1357AEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -2588,7 +2588,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2849,8 +2849,12 @@
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+      <c r="O3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Q3" s="6" t="s">
         <v>24</v>
       </c>
@@ -2912,8 +2916,12 @@
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="O4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -2969,8 +2977,12 @@
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
+      <c r="O5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
@@ -3026,8 +3038,12 @@
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+      <c r="O6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -3083,8 +3099,12 @@
       </c>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="O7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -3159,7 +3179,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
@@ -3172,7 +3192,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -3185,7 +3205,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -3211,7 +3231,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-11-14
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7C77A3-A7C1-4FF1-BA4C-619F1357AEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB6E618-F965-40C9-97A5-CCED4EE24783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -2588,7 +2588,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,9 +2922,15 @@
       <c r="P4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="Q4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
       <c r="V4" s="2"/>
@@ -2983,9 +2989,15 @@
       <c r="P5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
+      <c r="Q5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="2"/>
@@ -3044,9 +3056,15 @@
       <c r="P6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
+      <c r="Q6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
       <c r="V6" s="2"/>
@@ -3105,9 +3123,15 @@
       <c r="P7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
+      <c r="Q7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="2"/>
@@ -3196,7 +3220,7 @@
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -3205,11 +3229,11 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -3231,11 +3255,11 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-11-17
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB6E618-F965-40C9-97A5-CCED4EE24783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3444EE48-E501-4A82-B6FA-FFF1B7CC3BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -2588,7 +2588,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2866,7 +2866,9 @@
       </c>
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
-      <c r="V3" s="2"/>
+      <c r="V3" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
@@ -2933,7 +2935,9 @@
       </c>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
-      <c r="V4" s="2"/>
+      <c r="V4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
@@ -3000,7 +3004,9 @@
       </c>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
-      <c r="V5" s="2"/>
+      <c r="V5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
@@ -3067,7 +3073,9 @@
       </c>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
-      <c r="V6" s="2"/>
+      <c r="V6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
@@ -3134,7 +3142,9 @@
       </c>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
-      <c r="V7" s="2"/>
+      <c r="V7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
@@ -3216,7 +3226,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -3229,7 +3239,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -3255,7 +3265,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-11-19
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3444EE48-E501-4A82-B6FA-FFF1B7CC3BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745B0FD3-9CE2-4C3F-92D1-8EFDED4903F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1850" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -2587,8 +2587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42BC0F2-E7C0-48B4-8AB8-C4D08FDA0656}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2869,8 +2869,12 @@
       <c r="V3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
+      <c r="W3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="7"/>
@@ -2938,8 +2942,12 @@
       <c r="V4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
+      <c r="W4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="7"/>
@@ -3007,8 +3015,12 @@
       <c r="V5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
+      <c r="W5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="7"/>
@@ -3076,8 +3088,12 @@
       <c r="V6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
+      <c r="W6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="7"/>
@@ -3145,8 +3161,12 @@
       <c r="V7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
+      <c r="W7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="7"/>
@@ -3213,11 +3233,11 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -3226,7 +3246,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -3239,7 +3259,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -3265,7 +3285,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-11-21
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745B0FD3-9CE2-4C3F-92D1-8EFDED4903F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2684A9C9-1C72-463E-983F-D5C6C59C3159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1850" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -2588,7 +2588,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2875,8 +2875,12 @@
       <c r="X3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
+      <c r="Y3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="AA3" s="7"/>
       <c r="AB3" s="7"/>
       <c r="AC3" s="2"/>
@@ -2948,8 +2952,12 @@
       <c r="X4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
+      <c r="Y4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
       <c r="AC4" s="2"/>
@@ -3021,8 +3029,12 @@
       <c r="X5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
+      <c r="Y5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AA5" s="7"/>
       <c r="AB5" s="7"/>
       <c r="AC5" s="2"/>
@@ -3094,8 +3106,12 @@
       <c r="X6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
+      <c r="Y6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AA6" s="7"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="2"/>
@@ -3167,8 +3183,12 @@
       <c r="X7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
+      <c r="Y7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="2"/>
@@ -3246,7 +3266,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -3259,11 +3279,11 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -3285,7 +3305,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-11-24
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2684A9C9-1C72-463E-983F-D5C6C59C3159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB701552-9A42-4D7A-9521-DC8FA82DF356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -2587,7 +2587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42BC0F2-E7C0-48B4-8AB8-C4D08FDA0656}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Daily attendance update - 2025-11-25
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BCF8CA-A9C8-4588-8921-324809A216D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F84E2B5-571C-485E-9451-04CAAD818A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1865" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -2588,7 +2588,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2886,7 +2886,9 @@
       <c r="AC3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AD3" s="2"/>
+      <c r="AD3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
@@ -2965,7 +2967,9 @@
       <c r="AC4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AD4" s="2"/>
+      <c r="AD4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
@@ -3044,7 +3048,9 @@
       <c r="AC5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AD5" s="2"/>
+      <c r="AD5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
@@ -3123,7 +3129,9 @@
       <c r="AC6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AD6" s="2"/>
+      <c r="AD6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
@@ -3202,7 +3210,9 @@
       <c r="AC7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AD7" s="2"/>
+      <c r="AD7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
@@ -3263,7 +3273,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
@@ -3276,7 +3286,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -3289,7 +3299,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -3319,7 +3329,7 @@
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-11-26
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F84E2B5-571C-485E-9451-04CAAD818A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEBC25A-EA9D-4E7B-9832-AD5D386BF3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -2588,7 +2588,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AD7" sqref="AD7"/>
+      <selection activeCell="AG3" sqref="AG3:AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2889,9 +2889,15 @@
       <c r="AD3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-      <c r="AG3" s="2"/>
+      <c r="AE3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AH3" s="7"/>
       <c r="AI3" s="7"/>
     </row>
@@ -2970,9 +2976,15 @@
       <c r="AD4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
+      <c r="AE4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AH4" s="7"/>
       <c r="AI4" s="7"/>
     </row>
@@ -3051,9 +3063,15 @@
       <c r="AD5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AE5" s="2"/>
-      <c r="AF5" s="2"/>
-      <c r="AG5" s="2"/>
+      <c r="AE5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AH5" s="7"/>
       <c r="AI5" s="7"/>
     </row>
@@ -3132,9 +3150,15 @@
       <c r="AD6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AE6" s="2"/>
-      <c r="AF6" s="2"/>
-      <c r="AG6" s="2"/>
+      <c r="AE6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="AH6" s="7"/>
       <c r="AI6" s="7"/>
     </row>
@@ -3213,9 +3237,15 @@
       <c r="AD7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
+      <c r="AE7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AH7" s="7"/>
       <c r="AI7" s="7"/>
     </row>
@@ -3273,11 +3303,11 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
@@ -3286,11 +3316,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
@@ -3299,11 +3329,11 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
@@ -3325,11 +3355,11 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-12-02
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEBC25A-EA9D-4E7B-9832-AD5D386BF3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96AE18D-DD11-4DDE-A5B0-F68104D76CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="10" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="UV-WMS Admin September" sheetId="8" r:id="rId9"/>
     <sheet name="UV-WMS Admin October" sheetId="10" r:id="rId10"/>
     <sheet name="UV-WMS Admin November" sheetId="11" r:id="rId11"/>
+    <sheet name="UV-WMS Admin December" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -354,7 +355,37 @@
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2569,13 +2600,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2587,8 +2618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42BC0F2-E7C0-48B4-8AB8-C4D08FDA0656}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3:AG7"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V28" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3360,6 +3391,684 @@
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="B13:B17">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C623D-E1BD-4FE8-8DE5-A86BDEB0A522}">
+  <dimension ref="A1:AJ17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>45992</v>
+      </c>
+      <c r="G1" s="1">
+        <v>45993</v>
+      </c>
+      <c r="H1" s="1">
+        <v>45994</v>
+      </c>
+      <c r="I1" s="1">
+        <v>45995</v>
+      </c>
+      <c r="J1" s="1">
+        <v>45996</v>
+      </c>
+      <c r="K1" s="1">
+        <v>45997</v>
+      </c>
+      <c r="L1" s="1">
+        <v>45998</v>
+      </c>
+      <c r="M1" s="1">
+        <v>45999</v>
+      </c>
+      <c r="N1" s="1">
+        <v>46000</v>
+      </c>
+      <c r="O1" s="1">
+        <v>46001</v>
+      </c>
+      <c r="P1" s="1">
+        <v>46002</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>46003</v>
+      </c>
+      <c r="R1" s="1">
+        <v>46004</v>
+      </c>
+      <c r="S1" s="1">
+        <v>46005</v>
+      </c>
+      <c r="T1" s="1">
+        <v>46006</v>
+      </c>
+      <c r="U1" s="1">
+        <v>46007</v>
+      </c>
+      <c r="V1" s="1">
+        <v>46008</v>
+      </c>
+      <c r="W1" s="1">
+        <v>46009</v>
+      </c>
+      <c r="X1" s="1">
+        <v>46010</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>46011</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>46012</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>46013</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>46014</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>46015</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>46016</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>46017</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>46018</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>46019</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>46020</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>46021</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>46022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>35898</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2">
+        <v>33548</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44429</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
+        <v>36698</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45078</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <f>COUNTIF(F3:AI3,"WFO")</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <f>COUNTIF(F3:AI3,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <f>COUNTIF(F4:AI4,"WFO")</f>
+        <v>2</v>
+      </c>
+      <c r="C14" s="2">
+        <f>COUNTIF(F4:AI4,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2">
+        <f>COUNTIF(F5:AI5,"WFO")</f>
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <f>COUNTIF(F5:AI5,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2">
+        <f>COUNTIF(F6:AI6,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <f>COUNTIF(F6:AI6,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2">
+        <f>COUNTIF(F7:AI7,"WFO")</f>
+        <v>2</v>
+      </c>
+      <c r="C17" s="2">
+        <f>COUNTIF(F7:AI7,"WFH")</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4934,10 +5643,10 @@
     <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:B15">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5759,10 +6468,10 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6595,15 +7304,15 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="lessThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7400,13 +8109,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8235,13 +8944,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9053,13 +9762,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9869,13 +10578,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Daily attendance update - 2025-12-05
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96AE18D-DD11-4DDE-A5B0-F68104D76CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A2CF28-0ABE-4D91-8074-ABA83C7AC4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -2619,7 +2619,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V28" sqref="A1:XFD1048576"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3421,8 +3421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C623D-E1BD-4FE8-8DE5-A86BDEB0A522}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AE14" sqref="AE14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6:X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3735,9 +3735,15 @@
       <c r="G4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="2"/>
@@ -3797,9 +3803,15 @@
       <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="H5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="2"/>
@@ -3877,11 +3889,21 @@
       </c>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
+      <c r="T6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
       <c r="AA6" s="6" t="s">
@@ -3927,9 +3949,15 @@
       <c r="G7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="H7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="2"/>
@@ -4025,11 +4053,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -4038,11 +4066,11 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
@@ -4064,7 +4092,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-12-08
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A2CF28-0ABE-4D91-8074-ABA83C7AC4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A21CADC-36D6-433B-9034-B6E7507BA5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -3422,7 +3422,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6:X6"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3688,7 +3688,9 @@
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
-      <c r="M3" s="2"/>
+      <c r="M3" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -3746,7 +3748,9 @@
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="2"/>
+      <c r="M4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -3814,7 +3818,9 @@
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
-      <c r="M5" s="2"/>
+      <c r="M5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
@@ -3960,7 +3966,9 @@
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="2"/>
+      <c r="M7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
@@ -4053,7 +4061,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -4066,7 +4074,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -4092,7 +4100,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-12-09
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A21CADC-36D6-433B-9034-B6E7507BA5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E1581B-993D-44CA-ACEC-25C953569425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -3422,7 +3422,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="N3" sqref="N3:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3691,7 +3691,9 @@
       <c r="M3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="2"/>
+      <c r="N3" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -3751,7 +3753,9 @@
       <c r="M4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="2"/>
+      <c r="N4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -3821,7 +3825,9 @@
       <c r="M5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="2"/>
+      <c r="N5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -3969,7 +3975,9 @@
       <c r="M7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="2"/>
+      <c r="N7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -4061,7 +4069,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -4074,7 +4082,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -4100,7 +4108,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-12-10
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E1581B-993D-44CA-ACEC-25C953569425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB6AAB7-1204-44FD-88A5-AD40235BE2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -3422,7 +3422,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N7"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3694,7 +3694,9 @@
       <c r="N3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="2"/>
+      <c r="O3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="7"/>
@@ -3756,7 +3758,9 @@
       <c r="N4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="2"/>
+      <c r="O4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="7"/>
@@ -3828,7 +3832,9 @@
       <c r="N5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="2"/>
+      <c r="O5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="7"/>
@@ -3978,7 +3984,9 @@
       <c r="N7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="O7" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="7"/>
@@ -4056,7 +4064,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
@@ -4069,7 +4077,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -4082,7 +4090,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2025-12-11
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB6AAB7-1204-44FD-88A5-AD40235BE2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF920E43-CF66-4D4F-BA36-75CE38F62DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2006" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -3422,7 +3422,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,8 +3697,12 @@
       <c r="O3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="P3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
       <c r="T3" s="2"/>
@@ -3761,8 +3765,12 @@
       <c r="O4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+      <c r="P4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
       <c r="T4" s="2"/>
@@ -3835,7 +3843,9 @@
       <c r="O5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P5" s="2"/>
+      <c r="P5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
@@ -3987,8 +3997,12 @@
       <c r="O7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
+      <c r="P7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
       <c r="T7" s="2"/>
@@ -4068,7 +4082,7 @@
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -4081,7 +4095,7 @@
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -4094,7 +4108,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
@@ -4120,7 +4134,7 @@
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Daily attendance update - 2025-12-12
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF920E43-CF66-4D4F-BA36-75CE38F62DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BC1316-5DED-462F-9887-73D5562E8A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -3421,8 +3421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C623D-E1BD-4FE8-8DE5-A86BDEB0A522}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3768,8 +3768,8 @@
       <c r="P4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="5" t="s">
-        <v>17</v>
+      <c r="Q4" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
@@ -3846,7 +3846,9 @@
       <c r="P5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="2"/>
+      <c r="Q5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="2"/>
@@ -4091,11 +4093,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -4108,7 +4110,7 @@
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Daily attendance update - 2025-12-16
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BC1316-5DED-462F-9887-73D5562E8A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA0CF46-7FAB-4CA3-BEB5-013711A78E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="28">
   <si>
     <t>Person</t>
   </si>
@@ -3422,7 +3422,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="A4:D4"/>
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3705,8 +3705,12 @@
       </c>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="T3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
@@ -3773,8 +3777,12 @@
       </c>
       <c r="R4" s="7"/>
       <c r="S4" s="7"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
+      <c r="T4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
@@ -3851,8 +3859,12 @@
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
+      <c r="T5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
@@ -4007,8 +4019,12 @@
       </c>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
+      <c r="T7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
@@ -4080,7 +4096,7 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
@@ -4093,7 +4109,7 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
@@ -4106,7 +4122,7 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
@@ -4132,7 +4148,7 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>

</xml_diff>

<commit_message>
Daily attendance update - 2026-01-28
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA0CF46-7FAB-4CA3-BEB5-013711A78E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40480EE-84A0-4914-9676-256139B1B492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="11" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="12" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
   <sheets>
     <sheet name="UV-WMS Admin Jan" sheetId="9" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="UV-WMS Admin October" sheetId="10" r:id="rId10"/>
     <sheet name="UV-WMS Admin November" sheetId="11" r:id="rId11"/>
     <sheet name="UV-WMS Admin December" sheetId="12" r:id="rId12"/>
+    <sheet name="UV-WMS Admin January" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="29">
   <si>
     <t>Person</t>
   </si>
@@ -131,6 +132,9 @@
   </si>
   <si>
     <t>WFO count</t>
+  </si>
+  <si>
+    <t>HOLIDAY</t>
   </si>
 </sst>
 </file>
@@ -355,7 +359,37 @@
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2600,13 +2634,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3403,13 +3437,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3421,8 +3455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988C623D-E1BD-4FE8-8DE5-A86BDEB0A522}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4153,6 +4187,812 @@
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="B13:B17">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E71A27-DC0F-4421-B295-A887695B49EA}">
+  <dimension ref="A1:AJ17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>46023</v>
+      </c>
+      <c r="G1" s="1">
+        <v>46024</v>
+      </c>
+      <c r="H1" s="1">
+        <v>46025</v>
+      </c>
+      <c r="I1" s="1">
+        <v>46026</v>
+      </c>
+      <c r="J1" s="1">
+        <v>46027</v>
+      </c>
+      <c r="K1" s="1">
+        <v>46028</v>
+      </c>
+      <c r="L1" s="1">
+        <v>46029</v>
+      </c>
+      <c r="M1" s="1">
+        <v>46030</v>
+      </c>
+      <c r="N1" s="1">
+        <v>46031</v>
+      </c>
+      <c r="O1" s="1">
+        <v>46032</v>
+      </c>
+      <c r="P1" s="1">
+        <v>46033</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>46034</v>
+      </c>
+      <c r="R1" s="1">
+        <v>46035</v>
+      </c>
+      <c r="S1" s="1">
+        <v>46036</v>
+      </c>
+      <c r="T1" s="1">
+        <v>46037</v>
+      </c>
+      <c r="U1" s="1">
+        <v>46038</v>
+      </c>
+      <c r="V1" s="1">
+        <v>46039</v>
+      </c>
+      <c r="W1" s="1">
+        <v>46040</v>
+      </c>
+      <c r="X1" s="1">
+        <v>46041</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>46042</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>46043</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>46044</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>46045</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>46046</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>46047</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>46048</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>46049</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>46050</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>46051</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>46052</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>46053</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>35898</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="7"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2">
+        <v>33548</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="7"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44429</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="7"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
+        <v>36698</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="7"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45078</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="7"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <f>COUNTIF(F3:AI3,"WFO")</f>
+        <v>10</v>
+      </c>
+      <c r="C13" s="2">
+        <f>COUNTIF(F3:AI3,"WFH")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <f>COUNTIF(F4:AI4,"WFO")</f>
+        <v>8</v>
+      </c>
+      <c r="C14" s="2">
+        <f>COUNTIF(F4:AI4,"WFH")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2">
+        <f>COUNTIF(F5:AI5,"WFO")</f>
+        <v>11</v>
+      </c>
+      <c r="C15" s="2">
+        <f>COUNTIF(F5:AI5,"WFH")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2">
+        <f>COUNTIF(F6:AI6,"WFO")</f>
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <f>COUNTIF(F6:AI6,"WFH")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2">
+        <f>COUNTIF(F7:AI7,"WFO")</f>
+        <v>11</v>
+      </c>
+      <c r="C17" s="2">
+        <f>COUNTIF(F7:AI7,"WFH")</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -5727,10 +6567,10 @@
     <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:B15">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6552,10 +7392,10 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7388,15 +8228,15 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="lessThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8193,13 +9033,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9028,13 +9868,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9846,13 +10686,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10662,13 +11502,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Daily attendance update - 2026-02-02
</commit_message>
<xml_diff>
--- a/data/uv-wcs/App_Admin_UV-WCS.xlsx
+++ b/data/uv-wcs/App_Admin_UV-WCS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rethin\projects\wfo_tracker\data\uv-wcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40480EE-84A0-4914-9676-256139B1B492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70426563-985D-4E65-9FBF-6259971E304D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="12" xr2:uid="{BB3BFA0C-538F-411B-ABFF-D727D65D2D40}"/>
   </bookViews>
@@ -26,6 +26,7 @@
     <sheet name="UV-WMS Admin November" sheetId="11" r:id="rId11"/>
     <sheet name="UV-WMS Admin December" sheetId="12" r:id="rId12"/>
     <sheet name="UV-WMS Admin January" sheetId="13" r:id="rId13"/>
+    <sheet name="UV-WMS Admin Febu" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="29">
   <si>
     <t>Person</t>
   </si>
@@ -359,7 +360,37 @@
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2634,13 +2665,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3437,13 +3468,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4199,13 +4230,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4217,8 +4248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E71A27-DC0F-4421-B295-A887695B49EA}">
   <dimension ref="A1:AJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA7" sqref="AA7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AI5" sqref="AI5:AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4481,8 +4512,8 @@
       <c r="K3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>16</v>
+      <c r="L3" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>17</v>
@@ -4515,11 +4546,11 @@
       <c r="Y3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Z3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA3" s="5" t="s">
-        <v>17</v>
+      <c r="Z3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="AB3" s="5" t="s">
         <v>17</v>
@@ -4532,9 +4563,15 @@
       <c r="AF3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AG3" s="2"/>
-      <c r="AH3" s="2"/>
-      <c r="AI3" s="2"/>
+      <c r="AG3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AJ3" s="7"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
@@ -4570,8 +4607,8 @@
       <c r="L4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>17</v>
+      <c r="M4" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>17</v>
@@ -4581,17 +4618,17 @@
       <c r="Q4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R4" s="4" t="s">
-        <v>16</v>
+      <c r="R4" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>17</v>
+      <c r="T4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
@@ -4618,9 +4655,15 @@
       <c r="AF4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2"/>
-      <c r="AI4" s="2"/>
+      <c r="AG4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="AJ4" s="7"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
@@ -4642,19 +4685,19 @@
       <c r="F5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>16</v>
+      <c r="G5" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>16</v>
+      <c r="K5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>17</v>
@@ -4670,14 +4713,14 @@
       <c r="R5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>17</v>
+      <c r="S5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="V5" s="7"/>
       <c r="W5" s="7"/>
@@ -4704,9 +4747,15 @@
       <c r="AF5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AG5" s="2"/>
-      <c r="AH5" s="2"/>
-      <c r="AI5" s="2"/>
+      <c r="AG5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI5" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AJ5" s="7"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -4750,8 +4799,8 @@
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
-      <c r="Q6" s="4" t="s">
-        <v>16</v>
+      <c r="Q6" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="R6" s="5" t="s">
         <v>17</v>
@@ -4790,9 +4839,15 @@
       <c r="AF6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="2"/>
-      <c r="AI6" s="2"/>
+      <c r="AG6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI6" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AJ6" s="7"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -4876,9 +4931,15 @@
       <c r="AF7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
-      <c r="AI7" s="2"/>
+      <c r="AG7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI7" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="AJ7" s="7"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
@@ -4936,11 +4997,11 @@
       </c>
       <c r="B13" s="2">
         <f>COUNTIF(F3:AI3,"WFO")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2">
         <f>COUNTIF(F3:AI3,"WFH")</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -4949,11 +5010,11 @@
       </c>
       <c r="B14" s="2">
         <f>COUNTIF(F4:AI4,"WFO")</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2">
         <f>COUNTIF(F4:AI4,"WFH")</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -4962,11 +5023,11 @@
       </c>
       <c r="B15" s="2">
         <f>COUNTIF(F5:AI5,"WFO")</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2">
         <f>COUNTIF(F5:AI5,"WFH")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
@@ -4975,11 +5036,11 @@
       </c>
       <c r="B16" s="2">
         <f>COUNTIF(F6:AI6,"WFO")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2">
         <f>COUNTIF(F6:AI6,"WFH")</f>
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -4988,11 +5049,590 @@
       </c>
       <c r="B17" s="2">
         <f>COUNTIF(F7:AI7,"WFO")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2">
         <f>COUNTIF(F7:AI7,"WFH")</f>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="B13:B17">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F94C369-A483-4243-8B30-4AC8F8C2C920}">
+  <dimension ref="A1:AG17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE16" sqref="AE16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>46054</v>
+      </c>
+      <c r="G1" s="1">
+        <v>46055</v>
+      </c>
+      <c r="H1" s="1">
+        <v>46056</v>
+      </c>
+      <c r="I1" s="1">
+        <v>46057</v>
+      </c>
+      <c r="J1" s="1">
+        <v>46058</v>
+      </c>
+      <c r="K1" s="1">
+        <v>46059</v>
+      </c>
+      <c r="L1" s="1">
+        <v>46060</v>
+      </c>
+      <c r="M1" s="1">
+        <v>46061</v>
+      </c>
+      <c r="N1" s="1">
+        <v>46062</v>
+      </c>
+      <c r="O1" s="1">
+        <v>46063</v>
+      </c>
+      <c r="P1" s="1">
+        <v>46064</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>46065</v>
+      </c>
+      <c r="R1" s="1">
+        <v>46066</v>
+      </c>
+      <c r="S1" s="1">
+        <v>46067</v>
+      </c>
+      <c r="T1" s="1">
+        <v>46068</v>
+      </c>
+      <c r="U1" s="1">
+        <v>46069</v>
+      </c>
+      <c r="V1" s="1">
+        <v>46070</v>
+      </c>
+      <c r="W1" s="1">
+        <v>46071</v>
+      </c>
+      <c r="X1" s="1">
+        <v>46072</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>46073</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>46074</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>46075</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>46076</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>46077</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>46078</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>46079</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>46080</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>46081</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>35898</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="7"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2">
+        <v>33548</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="7"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44429</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="7"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
+        <v>36698</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="7"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45078</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="7"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <f>COUNTIF(F3:AG3,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <f>COUNTIF(F3:AG3,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <f>COUNTIF(F4:AG4,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <f>COUNTIF(F4:AG4,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2">
+        <f>COUNTIF(F5:AG5,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <f>COUNTIF(F5:AG5,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2">
+        <f>COUNTIF(F6:AG6,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="2">
+        <f>COUNTIF(F6:AG6,"WFH")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2">
+        <f>COUNTIF(F7:AG7,"WFO")</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="2">
+        <f>COUNTIF(F7:AG7,"WFH")</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6567,10 +7207,10 @@
     <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:B15">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7392,10 +8032,10 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8228,15 +8868,15 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B16">
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="lessThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9033,13 +9673,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9868,13 +10508,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10686,13 +11326,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11502,13 +12142,13 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B17">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThan">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
       <formula>12</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>